<commit_message>
Connected projected to PM and updated test plans. Added jenkins build file
</commit_message>
<xml_diff>
--- a/ProvarProject/templates/OppData.xlsx
+++ b/ProvarProject/templates/OppData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\provardx\ProvarProject\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrdai\git\provardx\ProvarProject\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FAE24E-0F85-4574-8662-0DE4084E8C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338F8672-2954-4EFC-B6D6-D8FF880A10E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4050" windowWidth="29040" windowHeight="15720" xr2:uid="{395EF198-ADA6-4C3E-8A86-9204763D8F7E}"/>
+    <workbookView xWindow="-27345" yWindow="4860" windowWidth="17880" windowHeight="6645" activeTab="1" xr2:uid="{395EF198-ADA6-4C3E-8A86-9204763D8F7E}"/>
   </bookViews>
   <sheets>
     <sheet name="OppData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +144,21 @@
   </si>
   <si>
     <t>Michael Testy 151</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
+  <si>
+    <t>list_amount &gt; 50000</t>
+  </si>
+  <si>
+    <t>business_unit = "Transportation"</t>
   </si>
 </sst>
 </file>
@@ -501,20 +517,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAE9A52-E786-498E-A66C-790DA550D8D9}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.1328125" customWidth="1"/>
-    <col min="2" max="2" width="22.1328125" customWidth="1"/>
-    <col min="3" max="3" width="18.796875" customWidth="1"/>
+    <col min="1" max="1" width="18.08984375" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,8 +541,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -535,8 +555,11 @@
       <c r="C2" s="1">
         <v>44682</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -546,8 +569,11 @@
       <c r="C3" s="1">
         <v>44683</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -558,7 +584,7 @@
         <v>44684</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -569,7 +595,7 @@
         <v>44685</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -580,7 +606,7 @@
         <v>44686</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -591,7 +617,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -602,7 +628,7 @@
         <v>44688</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -613,7 +639,7 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -624,7 +650,7 @@
         <v>44690</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -635,7 +661,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -646,7 +672,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -657,7 +683,7 @@
         <v>44693</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -668,7 +694,7 @@
         <v>44694</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -679,7 +705,7 @@
         <v>44695</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -690,7 +716,7 @@
         <v>44696</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -701,7 +727,7 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -712,7 +738,7 @@
         <v>44698</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -723,7 +749,7 @@
         <v>44699</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -734,7 +760,7 @@
         <v>44700</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -745,7 +771,7 @@
         <v>44701</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -756,7 +782,7 @@
         <v>44702</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -767,7 +793,7 @@
         <v>44703</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -778,7 +804,7 @@
         <v>44704</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -789,7 +815,7 @@
         <v>44705</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -800,7 +826,7 @@
         <v>44706</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -811,7 +837,7 @@
         <v>44707</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -822,7 +848,7 @@
         <v>44708</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -833,7 +859,7 @@
         <v>44709</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -844,7 +870,7 @@
         <v>44710</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -855,7 +881,7 @@
         <v>44711</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -870,4 +896,71 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DEC71A-8620-49CF-995D-BCD84679CF2A}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>